<commit_message>
Adding in Entity and Unit functionality and Text reading
</commit_message>
<xml_diff>
--- a/ProjectApopalypse_Unity/Excel/StreamingAssets.xlsx
+++ b/ProjectApopalypse_Unity/Excel/StreamingAssets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectApopalypse\ProjectApopalypse_Unity\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FB7577-6158-4895-8751-56C183621757}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892BD0B3-ABBF-4A9F-95DF-2F29B534C6D4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C1DB6C17-836D-4EFD-91EA-180EF797A563}"/>
   </bookViews>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Yolo</t>
-  </si>
-  <si>
-    <t>Test123</t>
-  </si>
-  <si>
-    <t>Cooper</t>
-  </si>
-  <si>
-    <t>Hunter</t>
   </si>
 </sst>
 </file>
@@ -388,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99749392-E020-4C4D-9E07-6A73761AA19C}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -401,21 +392,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>